<commit_message>
updated uploads folders except product
</commit_message>
<xml_diff>
--- a/requirements.xlsx
+++ b/requirements.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OnGoing\ashley-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF69224-5876-4B14-9051-01AD40D1D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47F1D7C-6D67-4E1E-92A4-D91632223321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="6900" windowWidth="13140" windowHeight="9915" activeTab="3" xr2:uid="{9B9954AE-27A8-4982-954F-66D15F794264}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{9B9954AE-27A8-4982-954F-66D15F794264}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Tasks" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Meeting Points" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
   <si>
     <t>User</t>
   </si>
@@ -341,6 +342,15 @@
   <si>
     <t>Reviews based ratings</t>
   </si>
+  <si>
+    <t>Store users FORM doesn't contain Store ID</t>
+  </si>
+  <si>
+    <t>cart post route is based on user ID params</t>
+  </si>
+  <si>
+    <t>product needs to be add new with update controller &amp; api endpoints</t>
+  </si>
 </sst>
 </file>
 
@@ -349,7 +359,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$]dd/mmm/yy;@" x16r2:formatCode16="[$-en-PK,1]dd/mmm/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,6 +407,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -437,7 +454,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -465,6 +482,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -472,6 +490,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$]dd/mmm/yy;@" x16r2:formatCode16="[$-en-PK,1]dd/mmm/yy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -491,14 +517,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$]dd/mmm/yy;@" x16r2:formatCode16="[$-en-PK,1]dd/mmm/yy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -617,8 +635,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F59570DF-D901-4A01-87C9-E40F604C6CC2}" name="Table1" displayName="Table1" ref="A1:D27" totalsRowShown="0">
   <autoFilter ref="A1:D27" xr:uid="{F59570DF-D901-4A01-87C9-E40F604C6CC2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5009B7BE-FA3E-42D1-A3A7-ADFDBE142F67}" name="Day" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{840CBA56-9D8F-4DAC-8324-B50671BAC3EA}" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5009B7BE-FA3E-42D1-A3A7-ADFDBE142F67}" name="Day" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{840CBA56-9D8F-4DAC-8324-B50671BAC3EA}" name="Date" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{92688EF5-C27C-455B-BB57-170276A463AF}" name="Task Completed"/>
     <tableColumn id="3" xr3:uid="{E7D883C0-BDB9-40F9-863F-399D7734E280}" name="Remarks"/>
   </tableColumns>
@@ -1279,10 +1297,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A4 A6:A11 A27 A20:A25 A13:A18">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Sun">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Sun">
       <formula>NOT(ISERROR(SEARCH("Sun",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Sat">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Sat">
       <formula>NOT(ISERROR(SEARCH("Sat",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1699,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F4ED56-B76B-4837-9857-BA2CEA8C1F28}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,4 +1767,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F8031F-1C6F-4D4F-8CA6-920E4708C59C}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="31.5" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="134.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A2" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A3" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>